<commit_message>
backend => API list: added signup API
</commit_message>
<xml_diff>
--- a/backend/routes/list of APIs.xlsx
+++ b/backend/routes/list of APIs.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Acadamics and Work\Work\SE Factory\Assignments\dating-website\backend\routes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA2F97D-B1CA-4B74-A5D4-C1BC66CE4173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="list of APIs" sheetId="1" r:id="rId1"/>
+    <sheet name="signup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,12 +25,73 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>/signup</t>
+  </si>
+  <si>
+    <t>given name</t>
+  </si>
+  <si>
+    <t>signup</t>
+  </si>
+  <si>
+    <t>returns json</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>email already registered</t>
+  </si>
+  <si>
+    <t>invalid email</t>
+  </si>
+  <si>
+    <t>user (data)</t>
+  </si>
+  <si>
+    <t>Route inputs</t>
+  </si>
+  <si>
+    <t>name, email, age, bio, picture, gender, favorite_gender, location, password</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -37,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -45,17 +113,261 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +378,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2877EDCF-31D0-4631-8260-94E9DFEAAC4B}" name="Table2" displayName="Table2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:D2" xr:uid="{2877EDCF-31D0-4631-8260-94E9DFEAAC4B}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{AED43AA0-C238-4BFD-A1E1-D54587F01106}" name="Route" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{F63C7925-12B2-4F43-A37C-4D65845BA4FD}" name="Route inputs" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EDE5F8D0-D4A7-4418-AFDA-38D299DA6167}" name="given name" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{ED01493C-E6BB-49FC-BF18-AA733A27A31E}" name="returns json" dataDxfId="1" dataCellStyle="Hyperlink"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +655,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" location="signup!A1" display="data" xr:uid="{4BE6AF86-233C-44A4-B515-52B25D8853D5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB3F465-023A-4146-9141-29AA62D37F1B}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
backend => Listing APIs: Added signin api
</commit_message>
<xml_diff>
--- a/backend/routes/list of APIs.xlsx
+++ b/backend/routes/list of APIs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Acadamics and Work\Work\SE Factory\Assignments\dating-website\backend\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA2F97D-B1CA-4B74-A5D4-C1BC66CE4173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106416D9-56E5-40C0-AD46-A8D49E8738A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list of APIs" sheetId="1" r:id="rId1"/>
     <sheet name="signup" sheetId="2" r:id="rId2"/>
+    <sheet name="signin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Route</t>
   </si>
@@ -52,13 +53,46 @@
     <t>invalid email</t>
   </si>
   <si>
-    <t>user (data)</t>
-  </si>
-  <si>
     <t>Route inputs</t>
   </si>
   <si>
     <t>name, email, age, bio, picture, gender, favorite_gender, location, password</t>
+  </si>
+  <si>
+    <t>/signin</t>
+  </si>
+  <si>
+    <t>email, password</t>
+  </si>
+  <si>
+    <t>signin</t>
+  </si>
+  <si>
+    <t>$user(data)</t>
+  </si>
+  <si>
+    <t>invalid password</t>
+  </si>
+  <si>
+    <t>Registration Succeeded</t>
+  </si>
+  <si>
+    <t>email not registered</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>array</t>
   </si>
 </sst>
 </file>
@@ -188,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -196,6 +230,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -381,8 +419,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2877EDCF-31D0-4631-8260-94E9DFEAAC4B}" name="Table2" displayName="Table2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:D2" xr:uid="{2877EDCF-31D0-4631-8260-94E9DFEAAC4B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2877EDCF-31D0-4631-8260-94E9DFEAAC4B}" name="Table2" displayName="Table2" ref="A1:D3" totalsRowShown="0" headerRowDxfId="5" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:D3" xr:uid="{2877EDCF-31D0-4631-8260-94E9DFEAAC4B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AED43AA0-C238-4BFD-A1E1-D54587F01106}" name="Route" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{F63C7925-12B2-4F43-A37C-4D65845BA4FD}" name="Route inputs" dataDxfId="3"/>
@@ -656,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -689,18 +727,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" location="signup!A1" display="data" xr:uid="{4BE6AF86-233C-44A4-B515-52B25D8853D5}"/>
+    <hyperlink ref="D3" location="signin!A1" display="data" xr:uid="{2CE93D7F-A35A-4688-8BEE-CB6017711872}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -711,31 +764,135 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB3F465-023A-4146-9141-29AA62D37F1B}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D9EB4C-792B-4EB6-9098-78EDCC8DC843}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>